<commit_message>
Change example in input_user.xlsx
</commit_message>
<xml_diff>
--- a/input_user.xlsx
+++ b/input_user.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SWAP\swap_wofost_users\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SWAP\swap_wofost_users_adv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B8B0B9-D131-45A5-B609-73A36225E77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F45F7E3-6DEE-4AE3-ACC7-205ECC52D7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -967,7 +967,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1013,19 +1015,19 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="6">
-        <v>51.138806000000002</v>
+        <v>51.198633000000001</v>
       </c>
       <c r="C2" s="6">
-        <v>4.0249769999999998</v>
+        <v>4.9204559999999997</v>
       </c>
       <c r="D2" s="7">
         <v>42370</v>
       </c>
       <c r="E2" s="8">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>

</xml_diff>

<commit_message>
Keep main swp file and crop file
</commit_message>
<xml_diff>
--- a/input_user.xlsx
+++ b/input_user.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SWAP\swap_wofost_users_adv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SWAP\swap_wofost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F45F7E3-6DEE-4AE3-ACC7-205ECC52D7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4DE83B-9EA8-4AFF-BBBC-79DEB5E4AF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -968,7 +968,7 @@
   <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>